<commit_message>
Se actualizan archivos de pruebas.
</commit_message>
<xml_diff>
--- a/Material para pruebas/Relacion de OP.xlsx
+++ b/Material para pruebas/Relacion de OP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aidm\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FA3197CE-2AE4-4DBD-AF72-A6C0F712A41E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1878CF2C-5334-4430-BAD6-4696F98B2841}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="180" windowWidth="20490" windowHeight="4815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Relación de Pedidos para Adquisición de Combustibles en Plantas de Venta y Terminales de PETROPERU S.A.</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>FECHA</t>
+  </si>
+  <si>
+    <t>dasdsa</t>
   </si>
 </sst>
 </file>
@@ -93,7 +96,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -196,7 +199,7 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
@@ -252,6 +255,15 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -260,15 +272,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -696,10 +699,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A4:L13"/>
+  <dimension ref="A4:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,18 +723,18 @@
   <sheetData>
     <row r="4" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
@@ -746,46 +749,70 @@
       <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:12" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
     </row>
-    <row r="10" spans="1:12" s="25" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="24"/>
+    <row r="10" spans="1:12" s="22" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>0</v>
+      </c>
+      <c r="B10" s="7">
+        <v>1</v>
+      </c>
+      <c r="C10" s="20">
+        <v>2</v>
+      </c>
+      <c r="D10" s="7">
+        <v>3</v>
+      </c>
+      <c r="E10" s="7">
+        <v>4</v>
+      </c>
+      <c r="F10" s="7">
+        <v>5</v>
+      </c>
+      <c r="G10" s="9">
+        <v>6</v>
+      </c>
+      <c r="H10" s="7">
+        <v>7</v>
+      </c>
+      <c r="I10" s="10">
+        <v>8</v>
+      </c>
+      <c r="J10" s="7">
+        <v>9</v>
+      </c>
+      <c r="K10" s="7">
+        <v>10</v>
+      </c>
+      <c r="L10" s="21">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
@@ -851,7 +878,7 @@
         <v>12</v>
       </c>
       <c r="I12" s="5">
-        <v>11189204566</v>
+        <v>11520192875</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>17</v>
@@ -887,7 +914,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="5">
-        <v>11189214187</v>
+        <v>11520174353</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>18</v>
@@ -895,6 +922,11 @@
       <c r="K13" s="3"/>
       <c r="L13" s="6">
         <v>42377</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E14" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>